<commit_message>
L3IP-103 #time 3h #implementaçao dos inserts das operaçoes do lameiro do moinho
</commit_message>
<xml_diff>
--- a/LAPR3-2022-Self-Assessment_v2.0.xlsx
+++ b/LAPR3-2022-Self-Assessment_v2.0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Dropbox\Biogoods_dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcram\OneDrive - Instituto Superior de Engenharia do Porto\ISEP\licenciatura-engenharia-informatica\ano-02\semestre-01\projeto-integrador\SEM-3-PI-2023-24-G11\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647D2368-A99F-40FA-BBF4-CCC5C4A16F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -23,7 +24,7 @@
   <definedNames>
     <definedName name="ItemEval">[1]!Table2[ItemEval]</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,6 +36,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="141">
   <si>
     <t>Fill the cells with a blue background</t>
   </si>
@@ -63,18 +66,6 @@
   </si>
   <si>
     <t>List A</t>
-  </si>
-  <si>
-    <t>Student 1</t>
-  </si>
-  <si>
-    <t>Student 2</t>
-  </si>
-  <si>
-    <t>Student 3</t>
-  </si>
-  <si>
-    <t>Student 4</t>
   </si>
   <si>
     <t>Student 5</t>
@@ -510,11 +501,17 @@
   <si>
     <t>LAPR3 Project Group and Self-assessment v4.0</t>
   </si>
+  <si>
+    <t>US LP01</t>
+  </si>
+  <si>
+    <t>US LP02</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -1244,169 +1241,9 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1452,7 +1289,7 @@
             <xdr14:cNvPr id="7" name="Ink 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84EA9176-AD5B-1E48-B9F9-F07080AA6832}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84EA9176-AD5B-1E48-B9F9-F07080AA6832}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1517,7 +1354,7 @@
             <xdr14:cNvPr id="14" name="Ink 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C11775C-AEBD-3D40-A3A9-CC45ED1B07E2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C11775C-AEBD-3D40-A3A9-CC45ED1B07E2}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1566,7 +1403,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Instructions"/>
@@ -1932,56 +1769,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.875" customWidth="1"/>
+    <col min="4" max="19" width="7.8984375" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6">
+        <v>11</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:20" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="65" t="s">
@@ -2003,24 +1842,23 @@
       <c r="S8" s="66"/>
       <c r="T8" s="67"/>
     </row>
-    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="105.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="42" t="str">
+      <c r="D9" s="42">
         <f>C10</f>
-        <v>Student 1</v>
-      </c>
-      <c r="E9" s="43" t="str">
-        <f>C11</f>
-        <v>Student 2</v>
-      </c>
-      <c r="F9" s="43" t="str">
+        <v>1211742</v>
+      </c>
+      <c r="E9" s="43">
+        <v>1221636</v>
+      </c>
+      <c r="F9" s="43">
         <f>C12</f>
-        <v>Student 3</v>
-      </c>
-      <c r="G9" s="43" t="str">
+        <v>1221638</v>
+      </c>
+      <c r="G9" s="43">
         <f>C13</f>
-        <v>Student 4</v>
+        <v>1201260</v>
       </c>
       <c r="H9" s="43" t="str">
         <f>C14</f>
@@ -2070,17 +1908,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
+      <c r="C10" s="37">
+        <v>1211742</v>
+      </c>
+      <c r="D10" s="36">
+        <v>4</v>
+      </c>
+      <c r="E10" s="38">
+        <v>5</v>
+      </c>
+      <c r="F10" s="39">
+        <v>5</v>
+      </c>
+      <c r="G10" s="39">
+        <v>5</v>
+      </c>
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
@@ -2092,20 +1938,28 @@
       <c r="P10" s="39"/>
       <c r="Q10" s="39"/>
       <c r="R10" s="37"/>
-      <c r="S10" s="50" t="e">
+      <c r="S10" s="50">
         <f>AVERAGE(D10:R10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="63"/>
-      <c r="C11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="8"/>
+      <c r="C11" s="8">
+        <v>1221636</v>
+      </c>
+      <c r="D11" s="9">
+        <v>5</v>
+      </c>
+      <c r="E11" s="36">
+        <v>5</v>
+      </c>
+      <c r="F11" s="35">
+        <v>5</v>
+      </c>
+      <c r="G11" s="8">
+        <v>5</v>
+      </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -2117,20 +1971,28 @@
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="10"/>
-      <c r="S11" s="51" t="e">
+      <c r="S11" s="51">
         <f t="shared" ref="S11:S24" si="0">AVERAGE(D11:R11)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="63"/>
-      <c r="C12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="35"/>
+      <c r="C12" s="8">
+        <v>1221638</v>
+      </c>
+      <c r="D12" s="8">
+        <v>4</v>
+      </c>
+      <c r="E12" s="9">
+        <v>4</v>
+      </c>
+      <c r="F12" s="36">
+        <v>4</v>
+      </c>
+      <c r="G12" s="35">
+        <v>5</v>
+      </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -2142,20 +2004,28 @@
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="10"/>
-      <c r="S12" s="51" t="e">
+      <c r="S12" s="51">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="63"/>
-      <c r="C13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="36"/>
+      <c r="C13" s="8">
+        <v>1201260</v>
+      </c>
+      <c r="D13" s="8">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8">
+        <v>5</v>
+      </c>
+      <c r="F13" s="9">
+        <v>5</v>
+      </c>
+      <c r="G13" s="36">
+        <v>5</v>
+      </c>
       <c r="H13" s="35"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -2167,15 +2037,15 @@
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="10"/>
-      <c r="S13" s="51" t="e">
+      <c r="S13" s="51">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="63"/>
       <c r="C14" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -2197,10 +2067,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="63"/>
       <c r="C15" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -2222,10 +2092,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="63"/>
       <c r="C16" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -2247,10 +2117,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="63"/>
       <c r="C17" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -2272,10 +2142,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="63"/>
       <c r="C18" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -2297,10 +2167,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="63"/>
       <c r="C19" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -2322,10 +2192,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="63"/>
       <c r="C20" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -2347,10 +2217,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="63"/>
       <c r="C21" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -2372,10 +2242,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="63"/>
       <c r="C22" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -2397,10 +2267,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="63"/>
       <c r="C23" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -2422,10 +2292,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="64"/>
       <c r="C24" s="40" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -2447,26 +2317,26 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="46" t="e">
+      <c r="D25" s="46">
         <f>AVERAGE(D10:D24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E25" s="46" t="e">
+        <v>4.5</v>
+      </c>
+      <c r="E25" s="46">
         <f t="shared" ref="E25:R25" si="1">AVERAGE(E10:E24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F25" s="46" t="e">
+        <v>4.75</v>
+      </c>
+      <c r="F25" s="46">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G25" s="46" t="e">
+        <v>4.75</v>
+      </c>
+      <c r="G25" s="46">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="H25" s="46" t="e">
         <f t="shared" si="1"/>
@@ -2514,72 +2384,72 @@
       </c>
       <c r="S25" s="53"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2588,7 +2458,7 @@
     <mergeCell ref="E8:T8"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:R24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:R24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$31:$A$36</formula1>
     </dataValidation>
   </dataValidations>
@@ -2598,40 +2468,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.09765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="68" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="68" t="s">
-        <v>36</v>
       </c>
       <c r="E3" s="11">
         <v>0</v>
@@ -2652,532 +2522,578 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="63"/>
       <c r="B4" s="71"/>
       <c r="C4" s="71"/>
       <c r="D4" s="69"/>
       <c r="E4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="J4" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="63"/>
       <c r="B5" s="71"/>
       <c r="C5" s="71"/>
       <c r="D5" s="69"/>
       <c r="E5" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="J5" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="23" t="s">
+    </row>
+    <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="29">
+        <v>1211742</v>
+      </c>
+      <c r="C6" s="29">
+        <v>5</v>
+      </c>
+      <c r="D6" s="60">
+        <v>4</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="31" t="s">
+    </row>
+    <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>1</v>
+      </c>
+      <c r="B7" s="29">
+        <v>1221636</v>
+      </c>
+      <c r="C7" s="29">
+        <v>3</v>
+      </c>
+      <c r="D7" s="60">
+        <v>4</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="32" t="s">
+      <c r="J7" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="14" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>1</v>
+      </c>
+      <c r="B8" s="29">
+        <v>1221638</v>
+      </c>
+      <c r="C8" s="29">
+        <v>4</v>
+      </c>
+      <c r="D8" s="60">
+        <v>4</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="J8" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J7" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="14" t="s">
+    </row>
+    <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>1</v>
+      </c>
+      <c r="B9" s="29">
+        <v>1211742</v>
+      </c>
+      <c r="C9" s="29">
+        <v>4</v>
+      </c>
+      <c r="D9" s="60">
+        <v>4</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="J9" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="14" t="s">
+    </row>
+    <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="29">
+        <v>1211742</v>
+      </c>
+      <c r="C10" s="29">
+        <v>4</v>
+      </c>
+      <c r="D10" s="60">
+        <v>4</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="J10" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+    </row>
+    <row r="11" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>2</v>
+      </c>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="60"/>
       <c r="E11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="J11" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+    </row>
+    <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>2</v>
+      </c>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="60"/>
       <c r="E12" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="J12" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+    </row>
+    <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>2</v>
+      </c>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="60"/>
       <c r="E13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="J13" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="60"/>
       <c r="E14" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="J14" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
       <c r="D15" s="60"/>
       <c r="E15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="7" t="s">
+      <c r="J15" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
       <c r="D16" s="60"/>
       <c r="E16" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="7" t="s">
+      <c r="J16" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
       <c r="D17" s="60"/>
       <c r="E17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="J17" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J17" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="60"/>
       <c r="E18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="7" t="s">
+      <c r="J18" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="60"/>
       <c r="E19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" s="7" t="s">
+      <c r="J19" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J19" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="60"/>
       <c r="E20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="7" t="s">
+      <c r="J20" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J20" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="60"/>
       <c r="E21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="7" t="s">
+      <c r="J21" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J21" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="60"/>
       <c r="E22" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="7" t="s">
+      <c r="J22" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J22" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
       <c r="D23" s="60"/>
       <c r="E23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G23" s="7" t="s">
+      <c r="J23" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J23" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="60"/>
       <c r="E24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="7" t="s">
+      <c r="J24" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J24" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="22"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54"/>
       <c r="D25" s="61"/>
       <c r="E25" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" s="23" t="s">
+      <c r="J25" s="33" t="s">
         <v>45</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="I25" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="J25" s="33" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -3187,96 +3103,16 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A3:A5"/>
   </mergeCells>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
+  <conditionalFormatting sqref="E6:J25">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$C6=E$3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
-      <formula>$C6=F$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
-      <formula>$C6=G$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
-    <cfRule type="expression" dxfId="13" priority="17" stopIfTrue="1">
-      <formula>$C6=H$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="12" priority="21" stopIfTrue="1">
-      <formula>$C6=I$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J6">
-    <cfRule type="expression" dxfId="11" priority="22" stopIfTrue="1">
-      <formula>$C6=J$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E17">
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
-      <formula>$C7=E$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F17">
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
-      <formula>$C7=F$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G17">
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
-      <formula>$C7=G$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7:H17">
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
-      <formula>$C7=H$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7:I17">
-    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
-      <formula>$C7=I$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:E25">
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
-      <formula>$C18=E$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18:F25">
-    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
-      <formula>$C18=F$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G18:G25">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
-      <formula>$C18=G$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18:H25">
-    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
-      <formula>$C18=H$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18:I25">
-    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
-      <formula>$C18=I$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J25">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>$C7=J$3</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C25" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$E$40:$J$40</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C17" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$E$3:$J$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3284,7 +3120,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'Group and Self Assessment'!$C$10:$C$24</xm:f>
           </x14:formula1>
@@ -3297,34 +3133,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.875" style="1"/>
+    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3341,29 +3177,29 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="20" t="str">
+        <v>46</v>
+      </c>
+      <c r="C3" s="20">
         <f>'Group and Self Assessment'!C10</f>
-        <v>Student 1</v>
-      </c>
-      <c r="D3" s="20" t="str">
+        <v>1211742</v>
+      </c>
+      <c r="D3" s="20">
         <f>'Group and Self Assessment'!C11</f>
-        <v>Student 2</v>
-      </c>
-      <c r="E3" s="20" t="str">
+        <v>1221636</v>
+      </c>
+      <c r="E3" s="20">
         <f>'Group and Self Assessment'!C12</f>
-        <v>Student 3</v>
-      </c>
-      <c r="F3" s="20" t="str">
+        <v>1221638</v>
+      </c>
+      <c r="F3" s="20">
         <f>'Group and Self Assessment'!C13</f>
-        <v>Student 4</v>
+        <v>1201260</v>
       </c>
       <c r="G3" s="20" t="str">
         <f>'Group and Self Assessment'!C14</f>
@@ -3437,23 +3273,31 @@
         <v>5</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" s="17">
         <v>0.1</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+      <c r="C4" s="25">
+        <v>5</v>
+      </c>
+      <c r="D4" s="25">
+        <v>5</v>
+      </c>
+      <c r="E4" s="25">
+        <v>4</v>
+      </c>
+      <c r="F4" s="25">
+        <v>5</v>
+      </c>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
@@ -3465,42 +3309,50 @@
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
       <c r="Q4" s="25"/>
-      <c r="R4" s="27" t="e">
+      <c r="R4" s="27">
         <f t="shared" ref="R4:R7" si="0">AVERAGE(C4:Q4)</f>
-        <v>#DIV/0!</v>
+        <v>4.75</v>
       </c>
       <c r="S4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="T4" s="7" t="s">
+      <c r="X4" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="X4" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B5" s="17">
         <v>0.2</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="C5" s="25">
+        <v>1</v>
+      </c>
+      <c r="D5" s="25">
+        <v>1</v>
+      </c>
+      <c r="E5" s="25">
+        <v>1</v>
+      </c>
+      <c r="F5" s="25">
+        <v>1</v>
+      </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
@@ -3512,42 +3364,50 @@
       <c r="O5" s="25"/>
       <c r="P5" s="25"/>
       <c r="Q5" s="25"/>
-      <c r="R5" s="27" t="e">
+      <c r="R5" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="S5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="W5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="X5" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="V5" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="W5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="X5" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="78" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B6" s="17">
         <v>0.5</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="C6" s="25">
+        <v>4</v>
+      </c>
+      <c r="D6" s="25">
+        <v>4</v>
+      </c>
+      <c r="E6" s="25">
+        <v>4</v>
+      </c>
+      <c r="F6" s="25">
+        <v>4</v>
+      </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -3559,42 +3419,50 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="25"/>
-      <c r="R6" s="27" t="e">
+      <c r="R6" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="S6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W6" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="T6" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="X6" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B7" s="17">
         <v>0.2</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="C7" s="25">
+        <v>4</v>
+      </c>
+      <c r="D7" s="25">
+        <v>3</v>
+      </c>
+      <c r="E7" s="25">
+        <v>3</v>
+      </c>
+      <c r="F7" s="25">
+        <v>3</v>
+      </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -3606,97 +3474,97 @@
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
       <c r="Q7" s="25"/>
-      <c r="R7" s="27" t="e">
+      <c r="R7" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.25</v>
       </c>
       <c r="S7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="W7" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="T7" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="U7" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="V7" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="X7" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8" s="18">
         <f>SUM(B4:B7)</f>
         <v>1</v>
       </c>
       <c r="C8" s="7">
-        <f>SUMPRODUCT(C4:C7,$B$4:$B$7)</f>
+        <f t="shared" ref="C8:Q8" si="1">SUMPRODUCT(C4:C7,$B$4:$B$7)</f>
+        <v>3.5</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="1"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="1"/>
+        <v>3.2</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="1"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D8" s="7">
-        <f>SUMPRODUCT(D4:D7,$B$4:$B$7)</f>
+      <c r="H8" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="7">
-        <f>SUMPRODUCT(E4:E7,$B$4:$B$7)</f>
+      <c r="I8" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="7">
-        <f>SUMPRODUCT(F4:F7,$B$4:$B$7)</f>
+      <c r="J8" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G8" s="7">
-        <f>SUMPRODUCT(G4:G7,$B$4:$B$7)</f>
+      <c r="K8" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H8" s="7">
-        <f>SUMPRODUCT(H4:H7,$B$4:$B$7)</f>
+      <c r="L8" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I8" s="7">
-        <f>SUMPRODUCT(I4:I7,$B$4:$B$7)</f>
+      <c r="M8" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="7">
-        <f>SUMPRODUCT(J4:J7,$B$4:$B$7)</f>
+      <c r="N8" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="7">
-        <f>SUMPRODUCT(K4:K7,$B$4:$B$7)</f>
+      <c r="O8" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L8" s="7">
-        <f>SUMPRODUCT(L4:L7,$B$4:$B$7)</f>
+      <c r="P8" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M8" s="7">
-        <f>SUMPRODUCT(M4:M7,$B$4:$B$7)</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="7">
-        <f>SUMPRODUCT(N4:N7,$B$4:$B$7)</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="7">
-        <f>SUMPRODUCT(O4:O7,$B$4:$B$7)</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="7">
-        <f>SUMPRODUCT(P4:P7,$B$4:$B$7)</f>
-        <v>0</v>
-      </c>
       <c r="Q8" s="7">
-        <f>SUMPRODUCT(Q4:Q7,$B$4:$B$7)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R8" s="27"/>
@@ -3709,69 +3577,69 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23">
         <f>C8/5*20</f>
+        <v>14</v>
+      </c>
+      <c r="D9" s="23">
+        <f t="shared" ref="D9:Q9" si="2">D8/5*20</f>
+        <v>13.200000000000001</v>
+      </c>
+      <c r="E9" s="23">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="F9" s="23">
+        <f t="shared" si="2"/>
+        <v>13.200000000000001</v>
+      </c>
+      <c r="G9" s="23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D9" s="23">
-        <f t="shared" ref="D9:Q9" si="1">D8/5*20</f>
+      <c r="H9" s="23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E9" s="23">
-        <f t="shared" si="1"/>
+      <c r="I9" s="23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F9" s="23">
-        <f t="shared" si="1"/>
+      <c r="J9" s="23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G9" s="23">
-        <f t="shared" si="1"/>
+      <c r="K9" s="23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H9" s="23">
-        <f t="shared" si="1"/>
+      <c r="L9" s="23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I9" s="23">
-        <f t="shared" si="1"/>
+      <c r="M9" s="23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J9" s="23">
-        <f t="shared" si="1"/>
+      <c r="N9" s="23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K9" s="23">
-        <f t="shared" si="1"/>
+      <c r="O9" s="23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L9" s="23">
-        <f t="shared" si="1"/>
+      <c r="P9" s="23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M9" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N9" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="Q9" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R9" s="28"/>
@@ -3784,13 +3652,13 @@
       <c r="Y9" s="23"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:Q7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:Q7" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>$S$3:$X$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3799,32 +3667,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="20.625" style="1" customWidth="1"/>
+    <col min="22" max="24" width="20.59765625" style="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.875" style="1"/>
+    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="13"/>
@@ -3841,28 +3709,28 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="20" t="str">
+        <v>46</v>
+      </c>
+      <c r="C3" s="20">
         <f>'Group and Self Assessment'!C10</f>
-        <v>Student 1</v>
-      </c>
-      <c r="D3" s="20" t="str">
+        <v>1211742</v>
+      </c>
+      <c r="D3" s="20">
         <f>'Group and Self Assessment'!C11</f>
-        <v>Student 2</v>
-      </c>
-      <c r="E3" s="20" t="str">
+        <v>1221636</v>
+      </c>
+      <c r="E3" s="20">
         <f>'Group and Self Assessment'!C12</f>
-        <v>Student 3</v>
-      </c>
-      <c r="F3" s="20" t="str">
+        <v>1221638</v>
+      </c>
+      <c r="F3" s="20">
         <f>'Group and Self Assessment'!C13</f>
-        <v>Student 4</v>
+        <v>1201260</v>
       </c>
       <c r="G3" s="20" t="str">
         <f>'Group and Self Assessment'!C14</f>
@@ -3936,23 +3804,31 @@
         <v>5</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B4" s="17">
         <v>0.1</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+      <c r="C4" s="25">
+        <v>5</v>
+      </c>
+      <c r="D4" s="25">
+        <v>2</v>
+      </c>
+      <c r="E4" s="25">
+        <v>3</v>
+      </c>
+      <c r="F4" s="25">
+        <v>3</v>
+      </c>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
@@ -3964,42 +3840,50 @@
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
       <c r="Q4" s="25"/>
-      <c r="R4" s="55" t="e">
+      <c r="R4" s="55">
         <f t="shared" ref="R4:R7" si="0">AVERAGE(C4:Q4)</f>
-        <v>#DIV/0!</v>
+        <v>3.25</v>
       </c>
       <c r="S4" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="T4" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="U4" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="V4" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="W4" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="T4" s="59" t="s">
+      <c r="X4" s="59" t="s">
         <v>85</v>
-      </c>
-      <c r="U4" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="V4" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="W4" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="X4" s="59" t="s">
-        <v>89</v>
       </c>
       <c r="Y4" s="56"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B5" s="17">
         <v>0.1</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="C5" s="25">
+        <v>5</v>
+      </c>
+      <c r="D5" s="25">
+        <v>4</v>
+      </c>
+      <c r="E5" s="25">
+        <v>4</v>
+      </c>
+      <c r="F5" s="25">
+        <v>4</v>
+      </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
@@ -4011,42 +3895,50 @@
       <c r="O5" s="25"/>
       <c r="P5" s="25"/>
       <c r="Q5" s="25"/>
-      <c r="R5" s="55" t="e">
+      <c r="R5" s="55">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4.25</v>
       </c>
       <c r="S5" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="T5" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="U5" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="V5" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="W5" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="T5" s="59" t="s">
+      <c r="X5" s="59" t="s">
         <v>92</v>
-      </c>
-      <c r="U5" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="V5" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="W5" s="59" t="s">
-        <v>95</v>
-      </c>
-      <c r="X5" s="59" t="s">
-        <v>96</v>
       </c>
       <c r="Y5" s="56"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B6" s="17">
         <v>0.05</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="C6" s="25">
+        <v>4</v>
+      </c>
+      <c r="D6" s="25">
+        <v>4</v>
+      </c>
+      <c r="E6" s="25">
+        <v>4</v>
+      </c>
+      <c r="F6" s="25">
+        <v>4</v>
+      </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -4058,42 +3950,50 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="25"/>
-      <c r="R6" s="55" t="e">
+      <c r="R6" s="55">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="S6" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="T6" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="U6" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="V6" s="59" t="s">
+        <v>97</v>
+      </c>
+      <c r="W6" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="T6" s="59" t="s">
+      <c r="X6" s="59" t="s">
         <v>99</v>
-      </c>
-      <c r="U6" s="59" t="s">
-        <v>100</v>
-      </c>
-      <c r="V6" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="W6" s="59" t="s">
-        <v>102</v>
-      </c>
-      <c r="X6" s="59" t="s">
-        <v>103</v>
       </c>
       <c r="Y6" s="56"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B7" s="17">
         <v>0.05</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="C7" s="25">
+        <v>3</v>
+      </c>
+      <c r="D7" s="25">
+        <v>4</v>
+      </c>
+      <c r="E7" s="25">
+        <v>4</v>
+      </c>
+      <c r="F7" s="25">
+        <v>4</v>
+      </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -4105,42 +4005,50 @@
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
       <c r="Q7" s="25"/>
-      <c r="R7" s="55" t="e">
+      <c r="R7" s="55">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.75</v>
       </c>
       <c r="S7" s="59" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="T7" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="U7" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="V7" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="W7" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="X7" s="59" t="s">
         <v>105</v>
-      </c>
-      <c r="U7" s="59" t="s">
-        <v>106</v>
-      </c>
-      <c r="V7" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="W7" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="X7" s="59" t="s">
-        <v>109</v>
       </c>
       <c r="Y7" s="56"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B8" s="17">
         <v>0.1</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="C8" s="25">
+        <v>3</v>
+      </c>
+      <c r="D8" s="25">
+        <v>2</v>
+      </c>
+      <c r="E8" s="25">
+        <v>3</v>
+      </c>
+      <c r="F8" s="25">
+        <v>3</v>
+      </c>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -4152,42 +4060,50 @@
       <c r="O8" s="25"/>
       <c r="P8" s="25"/>
       <c r="Q8" s="25"/>
-      <c r="R8" s="55" t="e">
+      <c r="R8" s="55">
         <f t="shared" ref="R8:R12" si="1">AVERAGE(C8:Q8)</f>
-        <v>#DIV/0!</v>
+        <v>2.75</v>
       </c>
       <c r="S8" s="59" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="T8" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="U8" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="V8" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="W8" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="X8" s="59" t="s">
         <v>111</v>
-      </c>
-      <c r="U8" s="59" t="s">
-        <v>112</v>
-      </c>
-      <c r="V8" s="59" t="s">
-        <v>113</v>
-      </c>
-      <c r="W8" s="59" t="s">
-        <v>114</v>
-      </c>
-      <c r="X8" s="59" t="s">
-        <v>115</v>
       </c>
       <c r="Y8" s="56"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B9" s="17">
         <v>0.05</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="C9" s="25">
+        <v>3</v>
+      </c>
+      <c r="D9" s="25">
+        <v>2</v>
+      </c>
+      <c r="E9" s="25">
+        <v>2</v>
+      </c>
+      <c r="F9" s="25">
+        <v>2</v>
+      </c>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
@@ -4199,38 +4115,46 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="25"/>
-      <c r="R9" s="55" t="e">
+      <c r="R9" s="55">
         <f t="shared" ref="R9:R11" si="2">AVERAGE(C9:Q9)</f>
-        <v>#DIV/0!</v>
+        <v>2.25</v>
       </c>
       <c r="S9" s="59" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="T9" s="59" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="U9" s="59"/>
       <c r="V9" s="59" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="W9" s="59"/>
       <c r="X9" s="59" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Y9" s="56"/>
       <c r="Z9" s="15"/>
     </row>
-    <row r="10" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B10" s="17">
         <v>0.1</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="C10" s="25">
+        <v>3</v>
+      </c>
+      <c r="D10" s="25">
+        <v>1</v>
+      </c>
+      <c r="E10" s="25">
+        <v>1</v>
+      </c>
+      <c r="F10" s="25">
+        <v>1</v>
+      </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
@@ -4242,42 +4166,50 @@
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
       <c r="Q10" s="25"/>
-      <c r="R10" s="55" t="e">
+      <c r="R10" s="55">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
       <c r="S10" s="59" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="T10" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="U10" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="V10" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="W10" s="59" t="s">
+        <v>121</v>
+      </c>
+      <c r="X10" s="59" t="s">
         <v>122</v>
-      </c>
-      <c r="U10" s="59" t="s">
-        <v>123</v>
-      </c>
-      <c r="V10" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="W10" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="X10" s="59" t="s">
-        <v>126</v>
       </c>
       <c r="Y10" s="56"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B11" s="17">
         <v>0.1</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="C11" s="25">
+        <v>4</v>
+      </c>
+      <c r="D11" s="25">
+        <v>3</v>
+      </c>
+      <c r="E11" s="25">
+        <v>3</v>
+      </c>
+      <c r="F11" s="25">
+        <v>2</v>
+      </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
@@ -4289,42 +4221,50 @@
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
       <c r="Q11" s="25"/>
-      <c r="R11" s="55" t="e">
+      <c r="R11" s="55">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="S11" s="59" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="T11" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="U11" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="V11" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="W11" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="X11" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="U11" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="V11" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="W11" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="X11" s="59" t="s">
-        <v>132</v>
       </c>
       <c r="Y11" s="56"/>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B12" s="17">
         <v>0.1</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+      <c r="C12" s="25">
+        <v>4</v>
+      </c>
+      <c r="D12" s="25">
+        <v>3</v>
+      </c>
+      <c r="E12" s="25">
+        <v>3</v>
+      </c>
+      <c r="F12" s="25">
+        <v>2</v>
+      </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -4336,42 +4276,50 @@
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
       <c r="Q12" s="25"/>
-      <c r="R12" s="55" t="e">
+      <c r="R12" s="55">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="S12" s="59" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="T12" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="U12" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="V12" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="W12" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="X12" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="U12" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="V12" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="W12" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="X12" s="59" t="s">
-        <v>132</v>
       </c>
       <c r="Y12" s="56"/>
       <c r="Z12" s="15"/>
     </row>
-    <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B13" s="17">
         <v>0.1</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="C13" s="25">
+        <v>5</v>
+      </c>
+      <c r="D13" s="25">
+        <v>5</v>
+      </c>
+      <c r="E13" s="25">
+        <v>5</v>
+      </c>
+      <c r="F13" s="25">
+        <v>5</v>
+      </c>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
@@ -4383,42 +4331,50 @@
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
       <c r="Q13" s="25"/>
-      <c r="R13" s="55" t="e">
+      <c r="R13" s="55">
         <f t="shared" ref="R13:R14" si="3">AVERAGE(C13:Q13)</f>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="S13" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="T13" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="U13" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="V13" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="W13" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="T13" s="59" t="s">
+      <c r="X13" s="59" t="s">
         <v>136</v>
-      </c>
-      <c r="U13" s="59" t="s">
-        <v>137</v>
-      </c>
-      <c r="V13" s="59" t="s">
-        <v>138</v>
-      </c>
-      <c r="W13" s="59" t="s">
-        <v>139</v>
-      </c>
-      <c r="X13" s="59" t="s">
-        <v>140</v>
       </c>
       <c r="Y13" s="56"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B14" s="17">
         <v>0.15</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
+      <c r="C14" s="25">
+        <v>4</v>
+      </c>
+      <c r="D14" s="25">
+        <v>3</v>
+      </c>
+      <c r="E14" s="25">
+        <v>3</v>
+      </c>
+      <c r="F14" s="25">
+        <v>3</v>
+      </c>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
@@ -4430,34 +4386,34 @@
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="25"/>
-      <c r="R14" s="55" t="e">
+      <c r="R14" s="55">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>3.25</v>
       </c>
       <c r="S14" s="59" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="T14" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="U14" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="V14" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="W14" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="X14" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="U14" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="V14" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="W14" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="X14" s="59" t="s">
-        <v>132</v>
       </c>
       <c r="Y14" s="56"/>
       <c r="Z14" s="15"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B15" s="18">
         <f>SUM(B4:B14)</f>
@@ -4465,19 +4421,19 @@
       </c>
       <c r="C15" s="7">
         <f>SUMPRODUCT(C4:C14,$B$4:$B$14)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" ref="D15:Q15" si="4">SUMPRODUCT(D4:D14,$B$4:$B$14)</f>
-        <v>0</v>
+        <v>2.95</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.1500000000000004</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.95</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="4"/>
@@ -4533,26 +4489,26 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23">
         <f>C15/5*20</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D16" s="23">
         <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
-        <v>0</v>
+        <v>11.8</v>
       </c>
       <c r="E16" s="23">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>12.600000000000001</v>
       </c>
       <c r="F16" s="23">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>11.8</v>
       </c>
       <c r="G16" s="23">
         <f t="shared" si="5"/>
@@ -4608,12 +4564,12 @@
       <c r="Y16" s="23"/>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:Q14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:Q14" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>$S$3:$X$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -4623,6 +4579,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4631,26 +4595,31 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
-    <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E82BD0DFFEA54847BE9781F1DBCFA3FB" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5129d64688598b451aff281771fab25">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a" xmlns:ns4="44ac372e-b264-4cba-b63b-83a010c5a6a2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fce63a6b29524334059c77e21a30d174" ns3:_="" ns4:_="">
+    <xsd:import namespace="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a"/>
+    <xsd:import namespace="44ac372e-b264-4cba-b63b-83a010c5a6a2"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4658,7 +4627,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -4671,48 +4640,86 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="_activity" ma:index="17" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="18" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="15" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="20" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="21" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="44ac372e-b264-4cba-b63b-83a010c5a6a2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="12" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -4815,13 +4822,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="44ac372e-b264-4cba-b63b-83a010c5a6a2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4829,14 +4847,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B687A809-3459-430D-93EA-BCBBCAA8A3A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a"/>
+    <ds:schemaRef ds:uri="44ac372e-b264-4cba-b63b-83a010c5a6a2"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -4845,20 +4864,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Diretório Sprint 3 adicionado
</commit_message>
<xml_diff>
--- a/LAPR3-2022-Self-Assessment_v2.0.xlsx
+++ b/LAPR3-2022-Self-Assessment_v2.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27123"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcram\OneDrive - Instituto Superior de Engenharia do Porto\ISEP\licenciatura-engenharia-informatica\ano-02\semestre-01\projeto-integrador\SEM-3-PI-2023-24-G11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myisepipp-my.sharepoint.com/personal/1211742_isep_ipp_pt/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647D2368-A99F-40FA-BBF4-CCC5C4A16F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E31A31C-5598-44D4-B55D-AAC24E1AD449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="ItemEval">[1]!Table2[ItemEval]</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="167">
+  <si>
+    <t>LAPR3 Project Group and Self-assessment v4.0</t>
+  </si>
   <si>
     <t>Fill the cells with a blue background</t>
   </si>
@@ -194,19 +197,100 @@
     <t>The students have exceeded expectations </t>
   </si>
   <si>
+    <t>USAC01</t>
+  </si>
+  <si>
     <t>The students  have exceeded expectations </t>
   </si>
   <si>
+    <t>USAC02</t>
+  </si>
+  <si>
+    <t>USAC03</t>
+  </si>
+  <si>
+    <t>USAC04</t>
+  </si>
+  <si>
+    <t>USAC05</t>
+  </si>
+  <si>
+    <t>USBD11</t>
+  </si>
+  <si>
+    <t>USBD12</t>
+  </si>
+  <si>
+    <t>USBD13</t>
+  </si>
+  <si>
+    <t>USBD14</t>
+  </si>
+  <si>
+    <t>USBD15</t>
+  </si>
+  <si>
+    <t>USBD16</t>
+  </si>
+  <si>
+    <t>USBD17</t>
+  </si>
+  <si>
+    <t>USBD18</t>
+  </si>
+  <si>
+    <t>USBD19</t>
+  </si>
+  <si>
+    <t>USBD20</t>
+  </si>
+  <si>
+    <t>USEI01</t>
+  </si>
+  <si>
+    <t>USEI02</t>
+  </si>
+  <si>
+    <t>USEI03</t>
+  </si>
+  <si>
+    <t>USEI04</t>
+  </si>
+  <si>
+    <t>USFA01</t>
+  </si>
+  <si>
+    <t>USFA02</t>
+  </si>
+  <si>
+    <t>USFA03</t>
+  </si>
+  <si>
+    <t>USLP03</t>
+  </si>
+  <si>
+    <t>USLP04</t>
+  </si>
+  <si>
+    <t>USLP05</t>
+  </si>
+  <si>
+    <t>USLP06</t>
+  </si>
+  <si>
+    <t>USLP07</t>
+  </si>
+  <si>
+    <t>USLP08</t>
+  </si>
+  <si>
+    <t>Project Development Self-Assessment</t>
+  </si>
+  <si>
+    <t>Rubric</t>
+  </si>
+  <si>
     <t>Weight</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Project Development Self-Assessment</t>
-  </si>
-  <si>
-    <t>Rubric</t>
   </si>
   <si>
     <t>Teacher
@@ -316,6 +400,9 @@
 data</t>
   </si>
   <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>Total (0-20)</t>
   </si>
   <si>
@@ -497,15 +584,6 @@
   </si>
   <si>
     <t>Overall Sprint management</t>
-  </si>
-  <si>
-    <t>LAPR3 Project Group and Self-assessment v4.0</t>
-  </si>
-  <si>
-    <t>US LP01</t>
-  </si>
-  <si>
-    <t>US LP02</t>
   </si>
 </sst>
 </file>
@@ -515,7 +593,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1241,7 +1319,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1773,58 +1851,58 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.8984375" customWidth="1"/>
+    <col min="4" max="19" width="7.875" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="21">
       <c r="A1" s="24" t="s">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" s="34" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:20" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="16.149999999999999" thickBot="1"/>
+    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="65" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F8" s="66"/>
       <c r="G8" s="66"/>
@@ -1842,7 +1920,7 @@
       <c r="S8" s="66"/>
       <c r="T8" s="67"/>
     </row>
-    <row r="9" spans="1:20" ht="105.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="42">
@@ -1850,15 +1928,16 @@
         <v>1211742</v>
       </c>
       <c r="E9" s="43">
+        <f>C11</f>
         <v>1221636</v>
       </c>
       <c r="F9" s="43">
         <f>C12</f>
-        <v>1221638</v>
+        <v>1201260</v>
       </c>
       <c r="G9" s="43">
         <f>C13</f>
-        <v>1201260</v>
+        <v>1221638</v>
       </c>
       <c r="H9" s="43" t="str">
         <f>C14</f>
@@ -1905,12 +1984,12 @@
         <v>Student 15</v>
       </c>
       <c r="S9" s="44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="B10" s="62" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="37">
         <v>1211742</v>
@@ -1943,7 +2022,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20">
       <c r="B11" s="63"/>
       <c r="C11" s="8">
         <v>1221636</v>
@@ -1976,19 +2055,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20">
       <c r="B12" s="63"/>
       <c r="C12" s="8">
-        <v>1221638</v>
+        <v>1201260</v>
       </c>
       <c r="D12" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F12" s="36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G12" s="35">
         <v>5</v>
@@ -2006,25 +2085,23 @@
       <c r="R12" s="10"/>
       <c r="S12" s="51">
         <f t="shared" si="0"/>
-        <v>4.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
       <c r="B13" s="63"/>
       <c r="C13" s="8">
-        <v>1201260</v>
+        <v>1221638</v>
       </c>
       <c r="D13" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="8">
-        <v>5</v>
-      </c>
-      <c r="F13" s="9">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F13" s="9"/>
       <c r="G13" s="36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H13" s="35"/>
       <c r="I13" s="8"/>
@@ -2039,13 +2116,13 @@
       <c r="R13" s="10"/>
       <c r="S13" s="51">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="16.149999999999999" thickBot="1">
       <c r="B14" s="63"/>
       <c r="C14" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -2067,10 +2144,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="16.149999999999999" thickBot="1">
       <c r="B15" s="63"/>
       <c r="C15" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -2092,10 +2169,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" ht="16.149999999999999" thickBot="1">
       <c r="B16" s="63"/>
       <c r="C16" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -2117,10 +2194,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="16.149999999999999" thickBot="1">
       <c r="B17" s="63"/>
       <c r="C17" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -2142,10 +2219,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="16.149999999999999" thickBot="1">
       <c r="B18" s="63"/>
       <c r="C18" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -2167,10 +2244,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" ht="16.149999999999999" thickBot="1">
       <c r="B19" s="63"/>
       <c r="C19" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -2192,10 +2269,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" ht="16.149999999999999" thickBot="1">
       <c r="B20" s="63"/>
       <c r="C20" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -2217,10 +2294,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" ht="16.149999999999999" thickBot="1">
       <c r="B21" s="63"/>
       <c r="C21" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -2242,10 +2319,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" ht="16.149999999999999" thickBot="1">
       <c r="B22" s="63"/>
       <c r="C22" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -2267,10 +2344,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="16.149999999999999" thickBot="1">
       <c r="B23" s="63"/>
       <c r="C23" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -2292,10 +2369,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" ht="16.149999999999999" thickBot="1">
       <c r="B24" s="64"/>
       <c r="C24" s="40" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -2317,10 +2394,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" ht="16.149999999999999" thickBot="1">
       <c r="B25" s="1"/>
       <c r="C25" s="45" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D25" s="46">
         <f>AVERAGE(D10:D24)</f>
@@ -2332,11 +2409,11 @@
       </c>
       <c r="F25" s="46">
         <f t="shared" si="1"/>
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="G25" s="46">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="H25" s="46" t="e">
         <f t="shared" si="1"/>
@@ -2384,72 +2461,72 @@
       </c>
       <c r="S25" s="53"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19">
       <c r="A27" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2470,38 +2547,38 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="A1" s="30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.149999999999999" thickBot="1"/>
+    <row r="3" spans="1:10">
       <c r="A3" s="62" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="70" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="68" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" s="11">
         <v>0</v>
@@ -2522,89 +2599,83 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="31.15">
       <c r="A4" s="63"/>
       <c r="B4" s="71"/>
       <c r="C4" s="71"/>
       <c r="D4" s="69"/>
       <c r="E4" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="47.45" thickBot="1">
       <c r="A5" s="63"/>
       <c r="B5" s="71"/>
       <c r="C5" s="71"/>
       <c r="D5" s="69"/>
       <c r="E5" s="22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="46.9">
+      <c r="A6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="F6" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="G6" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="H6" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="I6" s="32" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="B6" s="29">
-        <v>1211742</v>
-      </c>
-      <c r="C6" s="29">
-        <v>5</v>
-      </c>
-      <c r="D6" s="60">
-        <v>4</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>43</v>
-      </c>
       <c r="J6" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
-        <v>1</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="46.9">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="B7" s="29">
         <v>1221636</v>
@@ -2612,63 +2683,59 @@
       <c r="C7" s="29">
         <v>3</v>
       </c>
-      <c r="D7" s="60">
-        <v>4</v>
-      </c>
+      <c r="D7" s="60"/>
       <c r="E7" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="46.9">
+      <c r="A8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="29">
+        <v>1211742</v>
+      </c>
+      <c r="C8" s="29">
+        <v>4</v>
+      </c>
+      <c r="D8" s="60"/>
+      <c r="E8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
-        <v>1</v>
-      </c>
-      <c r="B8" s="29">
-        <v>1221638</v>
-      </c>
-      <c r="C8" s="29">
-        <v>4</v>
-      </c>
-      <c r="D8" s="60">
-        <v>4</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="I8" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14">
-        <v>1</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="46.9">
+      <c r="A9" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="B9" s="29">
         <v>1211742</v>
@@ -2676,424 +2743,706 @@
       <c r="C9" s="29">
         <v>4</v>
       </c>
-      <c r="D9" s="60">
-        <v>4</v>
-      </c>
+      <c r="D9" s="60"/>
       <c r="E9" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="46.9">
+      <c r="A10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="29">
+        <v>1221638</v>
+      </c>
+      <c r="C10" s="29">
+        <v>2</v>
+      </c>
+      <c r="D10" s="60"/>
+      <c r="E10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="29">
+      <c r="I10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="46.9">
+      <c r="A11" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="29">
         <v>1211742</v>
       </c>
-      <c r="C10" s="29">
-        <v>4</v>
-      </c>
-      <c r="D10" s="60">
-        <v>4</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
-        <v>2</v>
-      </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
+      <c r="C11" s="29">
+        <v>3</v>
+      </c>
       <c r="D11" s="60"/>
       <c r="E11" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J11" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
-        <v>2</v>
-      </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="46.9">
+      <c r="A12" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="29">
+        <v>1201260</v>
+      </c>
+      <c r="C12" s="29">
+        <v>4</v>
+      </c>
       <c r="D12" s="60"/>
       <c r="E12" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J12" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
-        <v>2</v>
-      </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="46.9">
+      <c r="A13" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="29">
+        <v>1201260</v>
+      </c>
+      <c r="C13" s="29">
+        <v>5</v>
+      </c>
       <c r="D13" s="60"/>
       <c r="E13" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J13" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="46.9">
+      <c r="A14" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="29">
+        <v>1201260</v>
+      </c>
+      <c r="C14" s="29">
+        <v>4</v>
+      </c>
       <c r="D14" s="60"/>
       <c r="E14" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J14" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="46.9">
+      <c r="A15" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1221638</v>
+      </c>
+      <c r="C15" s="29">
+        <v>3</v>
+      </c>
       <c r="D15" s="60"/>
       <c r="E15" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="46.9">
+      <c r="A16" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="29">
+        <v>1201260</v>
+      </c>
+      <c r="C16" s="29">
+        <v>4</v>
+      </c>
       <c r="D16" s="60"/>
       <c r="E16" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J16" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="46.9">
+      <c r="A17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="29">
+        <v>1221636</v>
+      </c>
+      <c r="C17" s="29">
+        <v>5</v>
+      </c>
       <c r="D17" s="60"/>
       <c r="E17" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J17" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="29"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="46.9">
+      <c r="A18" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="29">
+        <v>1211742</v>
+      </c>
       <c r="C18" s="29"/>
       <c r="D18" s="60"/>
       <c r="E18" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J18" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="29"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="46.9">
+      <c r="A19" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="29">
+        <v>1221638</v>
+      </c>
       <c r="C19" s="29"/>
       <c r="D19" s="60"/>
       <c r="E19" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J19" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="46.9">
+      <c r="A20" s="14" t="s">
+        <v>61</v>
+      </c>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="60"/>
       <c r="E20" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J20" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="46.9">
+      <c r="A21" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="60"/>
       <c r="E21" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J21" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
-      <c r="B22" s="29"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="46.9">
+      <c r="A22" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="29">
+        <v>1221638</v>
+      </c>
       <c r="C22" s="29"/>
       <c r="D22" s="60"/>
       <c r="E22" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J22" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="29"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="46.9">
+      <c r="A23" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="29">
+        <v>1221636</v>
+      </c>
       <c r="C23" s="29"/>
       <c r="D23" s="60"/>
       <c r="E23" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J23" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="46.9">
+      <c r="A24" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="29">
+        <v>1211742</v>
+      </c>
+      <c r="C24" s="29">
+        <v>4</v>
+      </c>
       <c r="D24" s="60"/>
       <c r="E24" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J24" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="22"/>
-      <c r="B25" s="54"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="46.9">
+      <c r="A25" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="54">
+        <v>1221636</v>
+      </c>
       <c r="C25" s="54"/>
       <c r="D25" s="61"/>
       <c r="E25" s="22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F25" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="47.45" thickBot="1">
+      <c r="A26" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="54">
+        <v>1211742</v>
+      </c>
+      <c r="C26" s="29">
+        <v>4</v>
+      </c>
+      <c r="D26" s="61"/>
+      <c r="E26" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="23" t="s">
+      <c r="F26" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="G26" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="23" t="s">
+      <c r="H26" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="J25" s="33" t="s">
-        <v>45</v>
+      <c r="I26" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J26" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="47.45" thickBot="1">
+      <c r="A27" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="29">
+        <v>1221638</v>
+      </c>
+      <c r="C27" s="54"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J27" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="47.45" thickBot="1">
+      <c r="A28" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J28" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="46.9">
+      <c r="A29" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="54">
+        <v>1211742</v>
+      </c>
+      <c r="C29" s="54"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J29" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="46.9">
+      <c r="A30" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="54">
+        <v>1221636</v>
+      </c>
+      <c r="C30" s="54"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J30" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="47.45" thickBot="1">
+      <c r="A31" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J31" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="47.45" thickBot="1">
+      <c r="A32" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J32" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="47.45" thickBot="1">
+      <c r="A33" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="29">
+        <v>1221638</v>
+      </c>
+      <c r="C33" s="54"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J33" s="33" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3103,16 +3452,17 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A3:A5"/>
   </mergeCells>
-  <conditionalFormatting sqref="E6:J25">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="E6:J33">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$C6=E$3</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C25" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C23 C25 C27:C33" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$E$40:$J$40</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C17" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C17 C24 C26" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$E$3:$J$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3124,7 +3474,7 @@
           <x14:formula1>
             <xm:f>'Group and Self Assessment'!$C$10:$C$24</xm:f>
           </x14:formula1>
-          <xm:sqref>B6:B25</xm:sqref>
+          <xm:sqref>B6:B33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3138,29 +3488,32 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.625" style="1" customWidth="1"/>
+    <col min="7" max="17" width="5.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.8984375" style="1"/>
+    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="21">
       <c r="A1" s="24" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3177,13 +3530,13 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="16.149999999999999" thickBot="1"/>
+    <row r="3" spans="1:26" ht="57">
       <c r="A3" s="19" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C3" s="20">
         <f>'Group and Self Assessment'!C10</f>
@@ -3195,11 +3548,11 @@
       </c>
       <c r="E3" s="20">
         <f>'Group and Self Assessment'!C12</f>
-        <v>1221638</v>
+        <v>1201260</v>
       </c>
       <c r="F3" s="20">
         <f>'Group and Self Assessment'!C13</f>
-        <v>1201260</v>
+        <v>1221638</v>
       </c>
       <c r="G3" s="20" t="str">
         <f>'Group and Self Assessment'!C14</f>
@@ -3246,7 +3599,7 @@
         <v>Student 15</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S3" s="26">
         <f>0</f>
@@ -3273,15 +3626,15 @@
         <v>5</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="62.45">
       <c r="A4" s="14" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="B4" s="17">
         <v>0.1</v>
@@ -3293,10 +3646,10 @@
         <v>5</v>
       </c>
       <c r="E4" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
@@ -3314,44 +3667,44 @@
         <v>4.75</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="124.9">
       <c r="A5" s="14" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="B5" s="17">
         <v>0.2</v>
       </c>
       <c r="C5" s="25">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5" s="25">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5" s="25">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F5" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -3366,32 +3719,32 @@
       <c r="Q5" s="25"/>
       <c r="R5" s="27">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4.25</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="78" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="78">
       <c r="A6" s="14" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="B6" s="17">
         <v>0.5</v>
@@ -3406,7 +3759,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -3421,32 +3774,32 @@
       <c r="Q6" s="25"/>
       <c r="R6" s="27">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3.25</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="93.6">
       <c r="A7" s="14" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="B7" s="17">
         <v>0.2</v>
@@ -3455,13 +3808,13 @@
         <v>4</v>
       </c>
       <c r="D7" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -3476,32 +3829,32 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="27">
         <f t="shared" si="0"/>
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26">
       <c r="A8" s="14" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="B8" s="18">
         <f>SUM(B4:B7)</f>
@@ -3509,19 +3862,19 @@
       </c>
       <c r="C8" s="7">
         <f t="shared" ref="C8:Q8" si="1">SUMPRODUCT(C4:C7,$B$4:$B$7)</f>
-        <v>3.5</v>
+        <v>4.3</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="1"/>
-        <v>3.3000000000000003</v>
+        <v>4.3</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="1"/>
-        <v>3.2</v>
+        <v>4.3</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="1"/>
-        <v>3.3000000000000003</v>
+        <v>2.1</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="1"/>
@@ -3577,26 +3930,26 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="16.149999999999999" thickBot="1">
       <c r="A9" s="22" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23">
         <f>C8/5*20</f>
-        <v>14</v>
+        <v>17.2</v>
       </c>
       <c r="D9" s="23">
         <f t="shared" ref="D9:Q9" si="2">D8/5*20</f>
-        <v>13.200000000000001</v>
+        <v>17.2</v>
       </c>
       <c r="E9" s="23">
         <f t="shared" si="2"/>
-        <v>12.8</v>
+        <v>17.2</v>
       </c>
       <c r="F9" s="23">
         <f t="shared" si="2"/>
-        <v>13.200000000000001</v>
+        <v>8.4</v>
       </c>
       <c r="G9" s="23">
         <f t="shared" si="2"/>
@@ -3652,7 +4005,7 @@
       <c r="Y9" s="23"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26">
       <c r="A10" s="5"/>
     </row>
   </sheetData>
@@ -3671,28 +4024,32 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.75" style="1" customWidth="1"/>
+    <col min="7" max="17" width="5.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="20.59765625" style="1" customWidth="1"/>
+    <col min="22" max="24" width="20.625" style="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.8984375" style="1"/>
+    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="21">
       <c r="A1" s="24" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="13"/>
@@ -3709,12 +4066,12 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="57">
       <c r="A3" s="19" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C3" s="20">
         <f>'Group and Self Assessment'!C10</f>
@@ -3726,11 +4083,11 @@
       </c>
       <c r="E3" s="20">
         <f>'Group and Self Assessment'!C12</f>
-        <v>1221638</v>
+        <v>1201260</v>
       </c>
       <c r="F3" s="20">
         <f>'Group and Self Assessment'!C13</f>
-        <v>1201260</v>
+        <v>1221638</v>
       </c>
       <c r="G3" s="20" t="str">
         <f>'Group and Self Assessment'!C14</f>
@@ -3777,7 +4134,7 @@
         <v>Student 15</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S3" s="57">
         <f>0</f>
@@ -3804,15 +4161,15 @@
         <v>5</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="144.75" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B4" s="17">
         <v>0.1</v>
@@ -3821,13 +4178,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="25">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E4" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F4" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
@@ -3842,32 +4199,32 @@
       <c r="Q4" s="25"/>
       <c r="R4" s="55">
         <f t="shared" ref="R4:R7" si="0">AVERAGE(C4:Q4)</f>
-        <v>3.25</v>
+        <v>4.75</v>
       </c>
       <c r="S4" s="59" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="T4" s="59" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="U4" s="59" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="V4" s="59" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="W4" s="59" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="X4" s="59" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="Y4" s="56"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="101.25" customHeight="1">
       <c r="A5" s="14" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="B5" s="17">
         <v>0.1</v>
@@ -3876,10 +4233,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="25">
         <v>4</v>
@@ -3897,32 +4254,32 @@
       <c r="Q5" s="25"/>
       <c r="R5" s="55">
         <f t="shared" si="0"/>
-        <v>4.25</v>
+        <v>4.75</v>
       </c>
       <c r="S5" s="59" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="T5" s="59" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="U5" s="59" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="V5" s="59" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="W5" s="59" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="X5" s="59" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="Y5" s="56"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="46.9">
       <c r="A6" s="14" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="B6" s="17">
         <v>0.05</v>
@@ -3934,10 +4291,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -3952,47 +4309,47 @@
       <c r="Q6" s="25"/>
       <c r="R6" s="55">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="S6" s="59" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="T6" s="59" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="U6" s="59" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="V6" s="59" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="W6" s="59" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="X6" s="59" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="Y6" s="56"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="46.9">
       <c r="A7" s="14" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="B7" s="17">
         <v>0.05</v>
       </c>
       <c r="C7" s="25">
+        <v>4</v>
+      </c>
+      <c r="D7" s="25">
+        <v>4</v>
+      </c>
+      <c r="E7" s="25">
+        <v>4</v>
+      </c>
+      <c r="F7" s="25">
         <v>3</v>
-      </c>
-      <c r="D7" s="25">
-        <v>4</v>
-      </c>
-      <c r="E7" s="25">
-        <v>4</v>
-      </c>
-      <c r="F7" s="25">
-        <v>4</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -4010,29 +4367,29 @@
         <v>3.75</v>
       </c>
       <c r="S7" s="59" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="T7" s="59" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="U7" s="59" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="V7" s="59" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="W7" s="59" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="X7" s="59" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="Y7" s="56"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="62.45">
       <c r="A8" s="14" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="B8" s="17">
         <v>0.1</v>
@@ -4041,13 +4398,13 @@
         <v>3</v>
       </c>
       <c r="D8" s="25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
@@ -4062,47 +4419,47 @@
       <c r="Q8" s="25"/>
       <c r="R8" s="55">
         <f t="shared" ref="R8:R12" si="1">AVERAGE(C8:Q8)</f>
-        <v>2.75</v>
+        <v>3.75</v>
       </c>
       <c r="S8" s="59" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="T8" s="59" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="U8" s="59" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="V8" s="59" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="W8" s="59" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="X8" s="59" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="Y8" s="56"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="62.45">
       <c r="A9" s="14" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="B9" s="17">
         <v>0.05</v>
       </c>
       <c r="C9" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9" s="25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" s="25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
@@ -4117,28 +4474,28 @@
       <c r="Q9" s="25"/>
       <c r="R9" s="55">
         <f t="shared" ref="R9:R11" si="2">AVERAGE(C9:Q9)</f>
-        <v>2.25</v>
+        <v>4</v>
       </c>
       <c r="S9" s="59" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="T9" s="59" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="U9" s="59"/>
       <c r="V9" s="59" t="s">
-        <v>115</v>
+        <v>144</v>
       </c>
       <c r="W9" s="59"/>
       <c r="X9" s="59" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="Y9" s="56"/>
       <c r="Z9" s="15"/>
     </row>
-    <row r="10" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="93.6">
       <c r="A10" s="14" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="B10" s="17">
         <v>0.1</v>
@@ -4147,10 +4504,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10" s="25">
         <v>1</v>
@@ -4168,44 +4525,44 @@
       <c r="Q10" s="25"/>
       <c r="R10" s="55">
         <f t="shared" si="2"/>
-        <v>1.5</v>
+        <v>2.75</v>
       </c>
       <c r="S10" s="59" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="T10" s="59" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="U10" s="59" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="V10" s="59" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="W10" s="59" t="s">
-        <v>121</v>
+        <v>150</v>
       </c>
       <c r="X10" s="59" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="Y10" s="56"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="31.15">
       <c r="A11" s="14" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="B11" s="17">
         <v>0.1</v>
       </c>
       <c r="C11" s="25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" s="25">
         <v>3</v>
       </c>
       <c r="E11" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="25">
         <v>2</v>
@@ -4226,29 +4583,29 @@
         <v>3</v>
       </c>
       <c r="S11" s="59" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="T11" s="59" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="U11" s="59" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="V11" s="59" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="W11" s="59" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
       <c r="X11" s="59" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="Y11" s="56"/>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="31.15">
       <c r="A12" s="14" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="B12" s="17">
         <v>0.1</v>
@@ -4257,13 +4614,13 @@
         <v>4</v>
       </c>
       <c r="D12" s="25">
+        <v>4</v>
+      </c>
+      <c r="E12" s="25">
+        <v>4</v>
+      </c>
+      <c r="F12" s="25">
         <v>3</v>
-      </c>
-      <c r="E12" s="25">
-        <v>3</v>
-      </c>
-      <c r="F12" s="25">
-        <v>2</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -4278,47 +4635,47 @@
       <c r="Q12" s="25"/>
       <c r="R12" s="55">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="S12" s="59" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="T12" s="59" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="U12" s="59" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="V12" s="59" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="W12" s="59" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
       <c r="X12" s="59" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="Y12" s="56"/>
       <c r="Z12" s="15"/>
     </row>
-    <row r="13" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="46.9">
       <c r="A13" s="14" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="B13" s="17">
         <v>0.1</v>
       </c>
       <c r="C13" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
@@ -4333,32 +4690,32 @@
       <c r="Q13" s="25"/>
       <c r="R13" s="55">
         <f t="shared" ref="R13:R14" si="3">AVERAGE(C13:Q13)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S13" s="59" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="T13" s="59" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="U13" s="59" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="V13" s="59" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="W13" s="59" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="X13" s="59" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="Y13" s="56"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="31.15">
       <c r="A14" s="14" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="B14" s="17">
         <v>0.15</v>
@@ -4367,10 +4724,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E14" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" s="25">
         <v>3</v>
@@ -4388,32 +4745,32 @@
       <c r="Q14" s="25"/>
       <c r="R14" s="55">
         <f t="shared" si="3"/>
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="S14" s="59" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="T14" s="59" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="U14" s="59" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="V14" s="59" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="W14" s="59" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
       <c r="X14" s="59" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="Y14" s="56"/>
       <c r="Z14" s="15"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26">
       <c r="A15" s="14" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="B15" s="18">
         <f>SUM(B4:B14)</f>
@@ -4421,19 +4778,19 @@
       </c>
       <c r="C15" s="7">
         <f>SUMPRODUCT(C4:C14,$B$4:$B$14)</f>
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" ref="D15:Q15" si="4">SUMPRODUCT(D4:D14,$B$4:$B$14)</f>
-        <v>2.95</v>
+        <v>3.9999999999999996</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="4"/>
-        <v>3.1500000000000004</v>
+        <v>4.25</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="4"/>
-        <v>2.95</v>
+        <v>3.25</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="4"/>
@@ -4489,26 +4846,26 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26">
       <c r="A16" s="22" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23">
         <f>C15/5*20</f>
-        <v>16</v>
+        <v>15.600000000000001</v>
       </c>
       <c r="D16" s="23">
         <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
-        <v>11.8</v>
+        <v>15.999999999999998</v>
       </c>
       <c r="E16" s="23">
         <f t="shared" si="5"/>
-        <v>12.600000000000001</v>
+        <v>17</v>
       </c>
       <c r="F16" s="23">
         <f t="shared" si="5"/>
-        <v>11.8</v>
+        <v>13</v>
       </c>
       <c r="G16" s="23">
         <f t="shared" si="5"/>
@@ -4564,7 +4921,7 @@
       <c r="Y16" s="23"/>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1">
       <c r="A17" s="5"/>
     </row>
   </sheetData>
@@ -4579,47 +4936,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E82BD0DFFEA54847BE9781F1DBCFA3FB" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5129d64688598b451aff281771fab25">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a" xmlns:ns4="44ac372e-b264-4cba-b63b-83a010c5a6a2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fce63a6b29524334059c77e21a30d174" ns3:_="" ns4:_="">
-    <xsd:import namespace="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a"/>
-    <xsd:import namespace="44ac372e-b264-4cba-b63b-83a010c5a6a2"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
+    <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:_activity" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4627,7 +4962,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -4640,86 +4975,48 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_activity" ma:index="17" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="15" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="18" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSystemTags" ma:index="20" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="21" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="44ac372e-b264-4cba-b63b-83a010c5a6a2" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SharingHintHash" ma:index="12" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -4822,46 +5119,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="44ac372e-b264-4cba-b63b-83a010c5a6a2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B687A809-3459-430D-93EA-BCBBCAA8A3A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c1feddaf-ff4f-4bf6-8204-bbbbb0a28c7a"/>
-    <ds:schemaRef ds:uri="44ac372e-b264-4cba-b63b-83a010c5a6a2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}"/>
 </file>
</xml_diff>